<commit_message>
plantillas vacias y cambios input fecha
</commit_message>
<xml_diff>
--- a/plantilla_lote_r_mercado.xlsx
+++ b/plantilla_lote_r_mercado.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naran\Entornos_virtuales\Pronosticos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naran\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26459A3E-B75A-47E4-87D9-D20177FF3063}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39A6D7F0-27BD-4CEC-AF03-AD8991AB7BF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8B61F6A3-CEA7-4A21-8727-FF0D76F946E5}"/>
+    <workbookView xWindow="5760" yWindow="3384" windowWidth="17280" windowHeight="8976" xr2:uid="{8B61F6A3-CEA7-4A21-8727-FF0D76F946E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -485,7 +485,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -521,351 +521,159 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="9">
-        <v>43770</v>
-      </c>
-      <c r="B2" s="2">
-        <v>9.2499999999999999E-2</v>
-      </c>
-      <c r="C2" s="2">
-        <v>3.8399999999999997E-2</v>
-      </c>
-      <c r="D2" s="3">
-        <v>3401.4730000000004</v>
-      </c>
-      <c r="E2" s="4">
-        <v>925148</v>
-      </c>
-      <c r="F2" s="5">
-        <v>55.17</v>
-      </c>
-      <c r="G2" s="6">
-        <v>23</v>
-      </c>
-      <c r="H2" s="6">
-        <v>2</v>
-      </c>
-      <c r="I2" s="6">
-        <v>46756</v>
-      </c>
+        <v>44348</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="9">
-        <v>43800</v>
-      </c>
-      <c r="B3" s="2">
-        <v>9.5299999999999996E-2</v>
-      </c>
-      <c r="C3" s="2">
-        <v>3.7999999999999999E-2</v>
-      </c>
-      <c r="D3" s="3">
-        <v>3378.050645161291</v>
-      </c>
-      <c r="E3" s="4">
-        <v>925148</v>
-      </c>
-      <c r="F3" s="5">
-        <v>61.06</v>
-      </c>
-      <c r="G3" s="6">
-        <v>25</v>
-      </c>
-      <c r="H3" s="6">
-        <v>2</v>
-      </c>
-      <c r="I3" s="6">
-        <v>58184</v>
-      </c>
+        <v>44378</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
-        <v>43831</v>
-      </c>
-      <c r="B4" s="2">
-        <v>0.12989999999999999</v>
-      </c>
-      <c r="C4" s="2">
-        <v>3.6200000000000003E-2</v>
-      </c>
-      <c r="D4" s="3">
-        <v>3311.1893548387097</v>
-      </c>
-      <c r="E4" s="4">
-        <v>980657</v>
-      </c>
-      <c r="F4" s="5">
-        <v>51.56</v>
-      </c>
-      <c r="G4" s="6">
-        <v>24</v>
-      </c>
-      <c r="H4" s="6">
-        <v>2</v>
-      </c>
-      <c r="I4" s="6">
-        <v>52046</v>
-      </c>
+        <v>44409</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="9">
-        <v>43862</v>
-      </c>
-      <c r="B5" s="2">
-        <v>0.122</v>
-      </c>
-      <c r="C5" s="2">
-        <v>3.7200000000000004E-2</v>
-      </c>
-      <c r="D5" s="3">
-        <v>3411.0527586206899</v>
-      </c>
-      <c r="E5" s="4">
-        <v>980657</v>
-      </c>
-      <c r="F5" s="5">
-        <v>44.76</v>
-      </c>
-      <c r="G5" s="6">
-        <v>24</v>
-      </c>
-      <c r="H5" s="6">
-        <v>0</v>
-      </c>
-      <c r="I5" s="6">
-        <v>55764</v>
-      </c>
+        <v>44440</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="9">
-        <v>43891</v>
-      </c>
-      <c r="B6" s="2">
-        <v>0.126</v>
-      </c>
-      <c r="C6" s="2">
-        <v>3.8599999999999995E-2</v>
-      </c>
-      <c r="D6" s="3">
-        <v>3877.0483870967751</v>
-      </c>
-      <c r="E6" s="4">
-        <v>980657</v>
-      </c>
-      <c r="F6" s="5">
-        <v>20.48</v>
-      </c>
-      <c r="G6" s="6">
-        <v>26</v>
-      </c>
-      <c r="H6" s="6">
-        <v>1</v>
-      </c>
-      <c r="I6" s="6">
-        <v>56352</v>
-      </c>
+        <v>44470</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
-        <v>43922</v>
-      </c>
-      <c r="B7" s="2">
-        <v>0.19800000000000001</v>
-      </c>
-      <c r="C7" s="2">
-        <v>3.5099999999999999E-2</v>
-      </c>
-      <c r="D7" s="3">
-        <v>3977.3933333333321</v>
-      </c>
-      <c r="E7" s="4">
-        <v>980657</v>
-      </c>
-      <c r="F7" s="5">
-        <v>19.559999999999999</v>
-      </c>
-      <c r="G7" s="6">
-        <v>24</v>
-      </c>
-      <c r="H7" s="6">
-        <v>2</v>
-      </c>
-      <c r="I7" s="6">
-        <v>53217</v>
-      </c>
+        <v>44501</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
-        <v>43952</v>
-      </c>
-      <c r="B8" s="2">
-        <v>0.21378491791541523</v>
-      </c>
-      <c r="C8" s="2">
-        <v>2.8500000000000001E-2</v>
-      </c>
-      <c r="D8" s="3">
-        <v>3858.1916129032265</v>
-      </c>
-      <c r="E8" s="4">
-        <v>980657</v>
-      </c>
-      <c r="F8" s="5">
-        <v>35.49</v>
-      </c>
-      <c r="G8" s="6">
-        <v>24</v>
-      </c>
-      <c r="H8" s="6">
-        <v>2</v>
-      </c>
-      <c r="I8" s="6">
-        <v>53995</v>
-      </c>
+        <v>44531</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
-        <v>43983</v>
-      </c>
-      <c r="B9" s="2">
-        <v>0.1981317683739327</v>
-      </c>
-      <c r="C9" s="2">
-        <v>2.1899999999999999E-2</v>
-      </c>
-      <c r="D9" s="3">
-        <v>3701.6043333333346</v>
-      </c>
-      <c r="E9" s="4">
-        <v>980657</v>
-      </c>
-      <c r="F9" s="5">
-        <v>39.270000000000003</v>
-      </c>
-      <c r="G9" s="6">
-        <v>24</v>
-      </c>
-      <c r="H9" s="6">
-        <v>2</v>
-      </c>
-      <c r="I9" s="6">
-        <v>50790</v>
-      </c>
+        <v>44562</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="9">
-        <v>44013</v>
-      </c>
-      <c r="B10" s="2">
-        <v>0.20223528686857242</v>
-      </c>
-      <c r="C10" s="2">
-        <v>1.9699999999999999E-2</v>
-      </c>
-      <c r="D10" s="3">
-        <v>3657.8667741935478</v>
-      </c>
-      <c r="E10" s="4">
-        <v>980657</v>
-      </c>
-      <c r="F10" s="5">
-        <v>40.270000000000003</v>
-      </c>
-      <c r="G10" s="6">
-        <v>25</v>
-      </c>
-      <c r="H10" s="6">
-        <v>2</v>
-      </c>
-      <c r="I10" s="6">
-        <v>51180</v>
-      </c>
+        <v>44593</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="9">
-        <v>44044</v>
-      </c>
-      <c r="B11" s="2">
-        <v>0.16757257612080015</v>
-      </c>
-      <c r="C11" s="2">
-        <v>1.8799999999999997E-2</v>
-      </c>
-      <c r="D11" s="3">
-        <v>3783.0258064516138</v>
-      </c>
-      <c r="E11" s="4">
-        <v>980657</v>
-      </c>
-      <c r="F11" s="5">
-        <v>42.61</v>
-      </c>
-      <c r="G11" s="6">
-        <v>24</v>
-      </c>
-      <c r="H11" s="6">
-        <v>2</v>
-      </c>
-      <c r="I11" s="6">
-        <v>44596</v>
-      </c>
+        <v>44621</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="9">
-        <v>44075</v>
-      </c>
-      <c r="B12" s="2">
-        <v>0.15770000000000001</v>
-      </c>
-      <c r="C12" s="2">
-        <v>1.9699999999999999E-2</v>
-      </c>
-      <c r="D12" s="3">
-        <v>3750.2153333333326</v>
-      </c>
-      <c r="E12" s="4">
-        <v>980657</v>
-      </c>
-      <c r="F12" s="5">
-        <v>40.22</v>
-      </c>
-      <c r="G12" s="6">
-        <v>26</v>
-      </c>
-      <c r="H12" s="6">
-        <v>0</v>
-      </c>
-      <c r="I12" s="6">
-        <v>55674</v>
-      </c>
+        <v>44652</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="9">
-        <v>44105</v>
-      </c>
-      <c r="B13" s="7">
-        <v>0.14699999999999999</v>
-      </c>
-      <c r="C13" s="7">
-        <v>1.7500000000000002E-2</v>
-      </c>
-      <c r="D13" s="8">
-        <v>3685.63</v>
-      </c>
-      <c r="E13" s="6">
-        <v>980657</v>
-      </c>
-      <c r="F13" s="6">
-        <v>38.31</v>
-      </c>
-      <c r="G13" s="6">
-        <v>25</v>
-      </c>
-      <c r="H13" s="6">
-        <v>1</v>
-      </c>
-      <c r="I13" s="6">
-        <v>55645</v>
-      </c>
+        <v>44682</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>